<commit_message>
cambios en la exportacion
</commit_message>
<xml_diff>
--- a/leads/steuerberater_kärnten_test.xlsx
+++ b/leads/steuerberater_kärnten_test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chistopherholder/Downloads/scraper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\web_scraping_cursos\outreach_automation\leads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C754EFB-C586-3340-8941-F5786B4B8432}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16104"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="344">
   <si>
     <t>Firma/Suchbegriff</t>
   </si>
@@ -1053,24 +1052,12 @@
   </si>
   <si>
     <t>Herr Wiegele Rupert</t>
-  </si>
-  <si>
-    <t>Herr Mag. Puri Michael</t>
-  </si>
-  <si>
-    <t>Frau Mag. Blazej Natascha</t>
-  </si>
-  <si>
-    <t>Herr Aicher Meinhard</t>
-  </si>
-  <si>
-    <t>Herr Hofer Thomas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1083,6 +1070,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1430,16 +1418,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1650,7 +1638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1718,7 +1706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1777,7 +1765,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1824,7 +1812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1880,7 +1868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1933,7 +1921,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1971,7 +1959,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2027,7 +2015,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2071,7 +2059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2192,7 +2180,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2245,7 +2233,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2298,7 +2286,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2360,7 +2348,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2410,7 +2398,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2460,7 +2448,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2510,7 +2498,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2551,7 +2539,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2604,7 +2592,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2693,7 +2681,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2737,7 +2725,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2796,7 +2784,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2831,7 +2819,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2881,7 +2869,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2934,7 +2922,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2981,502 +2969,490 @@
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
     </row>
-    <row r="114" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
     </row>
-    <row r="115" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
     </row>
-    <row r="116" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
     </row>
-    <row r="117" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
     </row>
-    <row r="118" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
     </row>
-    <row r="119" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
     </row>
-    <row r="120" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
     </row>
-    <row r="121" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
-      <c r="AZ122" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="123" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
     </row>
-    <row r="126" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
     </row>
-    <row r="128" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
     </row>
-    <row r="145" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
     </row>
-    <row r="146" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
     </row>
-    <row r="147" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
     </row>
-    <row r="148" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
     </row>
-    <row r="149" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
     </row>
-    <row r="150" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
     </row>
-    <row r="151" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
     </row>
-    <row r="152" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
     </row>
-    <row r="153" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
     </row>
-    <row r="154" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
     </row>
-    <row r="155" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
     </row>
-    <row r="156" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
     </row>
-    <row r="157" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
-      <c r="AZ157" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="158" spans="1:52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
     </row>
-    <row r="159" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
     </row>
-    <row r="160" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
     </row>
-    <row r="161" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
     </row>
-    <row r="162" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
     </row>
-    <row r="163" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
     </row>
-    <row r="164" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
     </row>
-    <row r="165" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
     </row>
-    <row r="166" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
     </row>
-    <row r="167" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
     </row>
-    <row r="168" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
     </row>
-    <row r="169" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
     </row>
-    <row r="170" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
-      <c r="AZ170" t="s">
-        <v>344</v>
-      </c>
-      <c r="BA170" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="171" spans="1:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
     </row>
-    <row r="172" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
     </row>
-    <row r="173" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
     </row>
-    <row r="174" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
     </row>
-    <row r="175" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
     </row>
-    <row r="176" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="3"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="3"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="3"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="3"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="3"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="3"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="3"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="3"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="3"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="3"/>
     </row>
   </sheetData>

</xml_diff>